<commit_message>
Added Change vCenter detailed function to waveEdit.py
</commit_message>
<xml_diff>
--- a/TestData/OneForAll/editVCenterData.xlsx
+++ b/TestData/OneForAll/editVCenterData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pranav Pawar\PycharmProjects\RMM_DataDriven\TestData\OneForAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D1D5F9-57E8-4EF6-932C-CE3C215FA622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEC58A8-6E04-47A7-B99D-061FEB3AFAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2856" yWindow="1032" windowWidth="18756" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2808" yWindow="1932" windowWidth="18756" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Wave Name</t>
   </si>
@@ -46,13 +46,31 @@
   </si>
   <si>
     <t>Routes</t>
+  </si>
+  <si>
+    <t>Host Names</t>
+  </si>
+  <si>
+    <t>Trial 3</t>
+  </si>
+  <si>
+    <t>hcm-cluster01</t>
+  </si>
+  <si>
+    <t>cwh-esx09.rackwareinc.lab</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>esx09-datastore3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +82,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -372,46 +396,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>